<commit_message>
updated all new files from mac
</commit_message>
<xml_diff>
--- a/Diet_builder/output_data/diet_plan_2300.xlsx
+++ b/Diet_builder/output_data/diet_plan_2300.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Venerdi" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Sabato" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Domenica" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Temporary_day" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +443,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Alimento</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -621,14 +622,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>yogurt 0% bianco</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>150</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>228.4 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>54.0 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>208.4 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Apporto di calorie totale:</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -642,7 +681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,7 +692,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Alimento</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -822,14 +861,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>yogurt 0% bianco</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>80</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>227.9 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>54.0 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>214.5 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Apporto di calorie totale:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -843,7 +920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1023,63 +1100,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Apporto proteico totale:</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>217.5</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-    </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Apporto di grassi totale:</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>46.1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>g</t>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>217.5 g</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Apporto di carboidrati totale:</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>229.4</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>g</t>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>46.1 g</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>229.4 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Apporto di calorie totale:</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>2300</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>kcal</t>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
         </is>
       </c>
     </row>
@@ -1345,14 +1410,235 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valore (g)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Milk pro budino (20g)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>banana</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bresaola</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cavolfiore</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>fiocchi latte (conad)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>gocce di cioccolato</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>insalata</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>miele</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>muesli conad</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>olio</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>pasta integrale</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>petto di pollo</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>proteine buone</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ricotta di mucca</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>riso</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>wasa</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>219.0 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>54.0 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>220.2 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Apporto di calorie totale:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1381,14 +1667,454 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valore (g)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Milk pro budino (20g)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>albume</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">barilla lenticchie </t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>bresaola</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cavolfiore</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>farina (normale)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fettine vitello</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>insalata</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>olio</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>proteine buone</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>riso</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sciroppo acero</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stracchino</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>uova</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>wasa</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>yogurt 0% bianco</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>216.6 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>51.8 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>220.5 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Apporto di calorie totale:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valore (g)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Milk pro budino (20g)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>barretta proteica</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bresaola</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cavolfiore</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>fiocchi avena</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>gocce di cioccolato</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>insalata</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>latte granarolo</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>olio</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>petto di pollo</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>riso</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>122.7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>salmone bollito</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>wasa</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>yogurt 0% bianco</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Apporto proteico totale:</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>216.5 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Apporto di grassi totale:</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>54.0 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Apporto di carboidrati totale:</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>219.7 g</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Apporto di calorie totale:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2300.0 kcal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>